<commit_message>
updata snc connector case
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-connector-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25335096-806F-4902-9B65-8843140C8E00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC1165C-37D6-4726-A011-BE4B60544594}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32811" yWindow="-129" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="179">
   <si>
     <t>name</t>
   </si>
@@ -553,9 +553,6 @@
   </si>
   <si>
     <t>bad request (condition includes rule key)</t>
-  </si>
-  <si>
-    <t>sql execution failed:Error while executing SQL</t>
   </si>
   <si>
     <t>snc-connector-differentTablesInTwoDb-7</t>
@@ -925,8 +922,8 @@
   <dimension ref="A1:M88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B89" sqref="B89"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M88" sqref="M88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.61328125" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
@@ -2954,7 +2951,7 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>175</v>
@@ -2969,15 +2966,15 @@
         <v>106601</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>164</v>
@@ -2989,10 +2986,7 @@
         <v>2</v>
       </c>
       <c r="L88" s="1">
-        <v>106103</v>
-      </c>
-      <c r="M88" s="1" t="s">
-        <v>176</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update test case due to use new SINAMICS_300_Log created on clickhouse which fixed snc portal issue
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-connector-test-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-with-comment\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CACE89-6F4E-4DD3-8CE0-9C15F7F1E27C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCFFE2A-FCEE-472B-81FA-EA01916BD594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -441,9 +441,6 @@
     <t>snc-connector-test-clickhouse-float-1</t>
   </si>
   <si>
-    <t>outputcurrent_actual_AI0='98.21999'</t>
-  </si>
-  <si>
     <t>snc-connector-test-clickhouse-time-1</t>
   </si>
   <si>
@@ -474,15 +471,9 @@
     <t>update_time&gt;'2021-06-03T04:50:19'</t>
   </si>
   <si>
-    <t>update_time&lt;'2021-06-03T04:50:19'</t>
-  </si>
-  <si>
     <t>update_time&gt;'2021-06-03 04:50:19'</t>
   </si>
   <si>
-    <t>update_time&lt;'2021-06-03 04:50:19'</t>
-  </si>
-  <si>
     <t>snc-connector-test-oracle-time-3</t>
   </si>
   <si>
@@ -562,6 +553,18 @@
   </si>
   <si>
     <t>do not support ruleKey value</t>
+  </si>
+  <si>
+    <t>outputcurrent_actual_AI0='160.66702'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>update_time&lt;'2021-09-06 13:33:58'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>update_time&lt;'2021-09-06T13:34:18'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -572,20 +575,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -922,23 +925,23 @@
   <dimension ref="A1:M88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A90" sqref="A90"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.61328125" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.15234375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.4609375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.61328125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="12.61328125" style="1"/>
-    <col min="6" max="6" width="17.53515625" style="1" customWidth="1"/>
-    <col min="7" max="12" width="12.61328125" style="1"/>
-    <col min="13" max="13" width="32.61328125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="12.61328125" style="1"/>
+    <col min="1" max="1" width="33.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="12.6640625" style="1"/>
+    <col min="6" max="6" width="17.5546875" style="1" customWidth="1"/>
+    <col min="7" max="12" width="12.6640625" style="1"/>
+    <col min="13" max="13" width="32.6640625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -979,7 +982,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
@@ -1000,7 +1003,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -1021,7 +1024,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
@@ -1048,7 +1051,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
@@ -1073,7 +1076,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>32</v>
       </c>
@@ -1096,7 +1099,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
@@ -1119,7 +1122,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>37</v>
       </c>
@@ -1142,7 +1145,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
@@ -1165,7 +1168,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
@@ -1188,7 +1191,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>40</v>
       </c>
@@ -1211,7 +1214,7 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>41</v>
       </c>
@@ -1234,7 +1237,7 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
@@ -1257,7 +1260,7 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
@@ -1280,7 +1283,7 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
@@ -1303,7 +1306,7 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>47</v>
       </c>
@@ -1326,7 +1329,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>52</v>
       </c>
@@ -1353,7 +1356,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>53</v>
       </c>
@@ -1380,7 +1383,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>54</v>
       </c>
@@ -1403,7 +1406,7 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>57</v>
       </c>
@@ -1428,7 +1431,7 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>58</v>
       </c>
@@ -1453,7 +1456,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>59</v>
       </c>
@@ -1478,7 +1481,7 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>50</v>
       </c>
@@ -1505,7 +1508,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>51</v>
       </c>
@@ -1532,7 +1535,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>61</v>
       </c>
@@ -1559,7 +1562,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>60</v>
       </c>
@@ -1586,7 +1589,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>62</v>
       </c>
@@ -1609,7 +1612,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>63</v>
       </c>
@@ -1632,7 +1635,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>64</v>
       </c>
@@ -1655,7 +1658,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>65</v>
       </c>
@@ -1678,7 +1681,7 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>66</v>
       </c>
@@ -1703,7 +1706,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>67</v>
       </c>
@@ -1728,7 +1731,7 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>68</v>
       </c>
@@ -1753,7 +1756,7 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>69</v>
       </c>
@@ -1778,7 +1781,7 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>70</v>
       </c>
@@ -1803,7 +1806,7 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>71</v>
       </c>
@@ -1828,7 +1831,7 @@
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>72</v>
       </c>
@@ -1853,7 +1856,7 @@
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>73</v>
       </c>
@@ -1878,7 +1881,7 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>74</v>
       </c>
@@ -1901,7 +1904,7 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>75</v>
       </c>
@@ -1924,7 +1927,7 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>76</v>
       </c>
@@ -1947,7 +1950,7 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>77</v>
       </c>
@@ -1970,7 +1973,7 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>78</v>
       </c>
@@ -1993,7 +1996,7 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>79</v>
       </c>
@@ -2016,7 +2019,7 @@
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>80</v>
       </c>
@@ -2039,7 +2042,7 @@
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>81</v>
       </c>
@@ -2062,12 +2065,12 @@
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>84</v>
@@ -2085,12 +2088,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>86</v>
@@ -2108,12 +2111,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>87</v>
@@ -2131,12 +2134,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>89</v>
@@ -2154,12 +2157,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>91</v>
@@ -2177,12 +2180,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>93</v>
@@ -2200,12 +2203,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>95</v>
@@ -2223,12 +2226,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>97</v>
@@ -2246,12 +2249,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>99</v>
@@ -2269,12 +2272,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>101</v>
@@ -2292,12 +2295,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>102</v>
@@ -2315,15 +2318,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>26</v>
@@ -2338,15 +2341,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>26</v>
@@ -2361,12 +2364,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>103</v>
@@ -2384,12 +2387,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>104</v>
@@ -2407,12 +2410,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>105</v>
@@ -2430,15 +2433,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>106</v>
@@ -2453,15 +2456,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>123</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>106</v>
@@ -2476,15 +2479,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>106</v>
@@ -2499,15 +2502,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>106</v>
@@ -2522,15 +2525,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>106</v>
@@ -2545,15 +2548,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>106</v>
@@ -2568,12 +2571,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>107</v>
@@ -2591,15 +2594,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>88</v>
@@ -2614,15 +2617,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>130</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>88</v>
@@ -2637,15 +2640,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>88</v>
@@ -2660,15 +2663,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>88</v>
@@ -2683,12 +2686,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>133</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>134</v>
@@ -2706,12 +2709,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>136</v>
@@ -2729,15 +2732,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>138</v>
+        <v>176</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>135</v>
@@ -2752,15 +2755,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>135</v>
@@ -2775,15 +2778,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>135</v>
@@ -2798,15 +2801,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>135</v>
@@ -2821,15 +2824,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>135</v>
@@ -2844,100 +2847,100 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="L81" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="L82" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="L83" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B81" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="L81" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A82" s="1" t="s">
+      <c r="B84" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="L84" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B82" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="L82" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A83" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="L83" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A84" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="L84" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A85" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="B85" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="L85" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H86" s="1">
         <v>1</v>
@@ -2949,35 +2952,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="L87" s="1">
         <v>106601</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H88" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
fix snc-test failed case due to data change in clcikhouse
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-connector-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-with-comment\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCFFE2A-FCEE-472B-81FA-EA01916BD594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B772948-0C80-4955-836F-819A77CCD685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -555,15 +555,15 @@
     <t>do not support ruleKey value</t>
   </si>
   <si>
-    <t>outputcurrent_actual_AI0='160.66702'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>update_time&lt;'2021-09-06 13:33:58'</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>update_time&lt;'2021-09-06T13:34:18'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>outputcurrent_actual_AI0='129.68036'</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -926,7 +926,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C80" sqref="C80"/>
+      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2740,7 +2740,7 @@
         <v>159</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>135</v>
@@ -2786,7 +2786,7 @@
         <v>159</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>135</v>
@@ -2832,7 +2832,7 @@
         <v>159</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>135</v>

</xml_diff>

<commit_message>
modify test case for connector when name is not present
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-connector-test-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24043799-4535-4FBE-AEE2-48D1A61C9B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E985E9-46E9-49DD-8679-8FE5A1D3D352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32811" yWindow="-129" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -564,7 +564,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>[add domain entities for mapping success] info</t>
+    <t>External configuration service is unavailable</t>
   </si>
 </sst>
 </file>
@@ -924,24 +924,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.69140625" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.07421875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.4609375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.69140625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="12.69140625" style="1"/>
-    <col min="6" max="6" width="17.53515625" style="1" customWidth="1"/>
-    <col min="7" max="12" width="12.69140625" style="1"/>
-    <col min="13" max="13" width="32.69140625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="12.69140625" style="1"/>
+    <col min="1" max="1" width="33.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="12.6640625" style="1"/>
+    <col min="6" max="6" width="17.5546875" style="1" customWidth="1"/>
+    <col min="7" max="12" width="12.6640625" style="1"/>
+    <col min="13" max="13" width="32.6640625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -982,7 +982,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -1003,7 +1003,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
@@ -1024,7 +1024,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
@@ -1099,7 +1099,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>32</v>
       </c>
@@ -1122,7 +1122,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>36</v>
       </c>
@@ -1145,7 +1145,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>37</v>
       </c>
@@ -1168,7 +1168,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>38</v>
       </c>
@@ -1191,7 +1191,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -1214,7 +1214,7 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
@@ -1237,7 +1237,7 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>41</v>
       </c>
@@ -1260,7 +1260,7 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
@@ -1283,7 +1283,7 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>44</v>
       </c>
@@ -1306,7 +1306,7 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>46</v>
       </c>
@@ -1329,7 +1329,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>51</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>52</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>53</v>
       </c>
@@ -1406,7 +1406,7 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>56</v>
       </c>
@@ -1431,7 +1431,7 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>57</v>
       </c>
@@ -1456,7 +1456,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>58</v>
       </c>
@@ -1481,7 +1481,7 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>49</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>50</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>60</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>59</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>61</v>
       </c>
@@ -1612,7 +1612,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>62</v>
       </c>
@@ -1635,7 +1635,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>63</v>
       </c>
@@ -1658,7 +1658,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>64</v>
       </c>
@@ -1681,7 +1681,7 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>65</v>
       </c>
@@ -1706,7 +1706,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>66</v>
       </c>
@@ -1731,7 +1731,7 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>67</v>
       </c>
@@ -1756,7 +1756,7 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>68</v>
       </c>
@@ -1781,7 +1781,7 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>69</v>
       </c>
@@ -1806,7 +1806,7 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>70</v>
       </c>
@@ -1831,7 +1831,7 @@
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>71</v>
       </c>
@@ -1856,7 +1856,7 @@
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>72</v>
       </c>
@@ -1881,7 +1881,7 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>73</v>
       </c>
@@ -1904,7 +1904,7 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>74</v>
       </c>
@@ -1927,7 +1927,7 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>75</v>
       </c>
@@ -1950,7 +1950,7 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>76</v>
       </c>
@@ -1973,7 +1973,7 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>77</v>
       </c>
@@ -1996,7 +1996,7 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>78</v>
       </c>
@@ -2019,7 +2019,7 @@
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>79</v>
       </c>
@@ -2042,7 +2042,7 @@
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>80</v>
       </c>
@@ -2065,7 +2065,7 @@
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>107</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>108</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>109</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>110</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>111</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>112</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>113</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>114</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>115</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>116</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>117</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>118</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>148</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>149</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>119</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>120</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>121</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>122</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>123</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>124</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>125</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>126</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>127</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>128</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>129</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>130</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>131</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>132</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>141</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>136</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>137</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>138</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>139</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>140</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>161</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>162</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>163</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>164</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>165</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>168</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>172</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>173</v>
       </c>

</xml_diff>

<commit_message>
update test cases after use latest dev images investigation
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-connector-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-backup\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6B4218-0227-416E-B350-774241A54CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2323047D-BA9A-44BA-9BCB-80F278685BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="182">
   <si>
     <t>name</t>
   </si>
@@ -465,12 +465,6 @@
     <t>IgnoreShortages=true</t>
   </si>
   <si>
-    <t>update_time&gt;'2021-06-03T04:50:19'</t>
-  </si>
-  <si>
-    <t>update_time&gt;'2021-06-03 04:50:19'</t>
-  </si>
-  <si>
     <t>snc-connector-test-oracle-time-3</t>
   </si>
   <si>
@@ -534,9 +528,6 @@
     <t>snc-connector-differentTablesInTwoDb-6</t>
   </si>
   <si>
-    <t>plant_owner=3</t>
-  </si>
-  <si>
     <t>location,-description</t>
   </si>
   <si>
@@ -547,9 +538,6 @@
   </si>
   <si>
     <t>snc-connector-differentTablesInTwoDb-8</t>
-  </si>
-  <si>
-    <t>do not support ruleKey value</t>
   </si>
   <si>
     <t>update_time&lt;'2021-09-06 13:33:58'</t>
@@ -564,7 +552,34 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>This entity 12321 is not found in domain [iEMS].</t>
+    <t>This entity 12321 is not found in domain [complexjson].</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bad request  (greater than the max records)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The number of reply records is greater than the max records</t>
+  </si>
+  <si>
+    <t>The number of reply records is greater than the max records</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>update_time&lt;'2021-06-03 04:50:19'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>update_time&gt;'2022-04-23T04:50:19'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>plant_owner=3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>do not support ruleKey value</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -925,14 +940,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87:XFD87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="39.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.6640625" style="1" customWidth="1"/>
     <col min="4" max="5" width="12.6640625" style="1"/>
@@ -1074,7 +1089,7 @@
         <v>108002</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2071,7 +2086,7 @@
         <v>107</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>83</v>
@@ -2094,7 +2109,7 @@
         <v>108</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>85</v>
@@ -2117,7 +2132,7 @@
         <v>109</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>86</v>
@@ -2140,7 +2155,7 @@
         <v>110</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>88</v>
@@ -2163,7 +2178,7 @@
         <v>111</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>90</v>
@@ -2186,7 +2201,7 @@
         <v>112</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>92</v>
@@ -2209,7 +2224,7 @@
         <v>113</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>94</v>
@@ -2232,7 +2247,7 @@
         <v>114</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>96</v>
@@ -2255,7 +2270,7 @@
         <v>115</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>98</v>
@@ -2278,7 +2293,7 @@
         <v>116</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>100</v>
@@ -2301,7 +2316,7 @@
         <v>117</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>101</v>
@@ -2324,10 +2339,10 @@
         <v>118</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>25</v>
@@ -2344,13 +2359,13 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>25</v>
@@ -2367,10 +2382,10 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>102</v>
@@ -2393,7 +2408,7 @@
         <v>119</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>103</v>
@@ -2416,7 +2431,7 @@
         <v>120</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>104</v>
@@ -2439,7 +2454,7 @@
         <v>121</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>142</v>
@@ -2462,7 +2477,7 @@
         <v>122</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>143</v>
@@ -2480,12 +2495,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>123</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>144</v>
@@ -2503,12 +2518,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>145</v>
@@ -2526,15 +2541,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>105</v>
@@ -2549,15 +2564,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>105</v>
@@ -2572,12 +2587,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>106</v>
@@ -2595,15 +2610,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>87</v>
@@ -2618,15 +2633,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>87</v>
@@ -2641,15 +2656,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>130</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>87</v>
@@ -2664,15 +2679,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>87</v>
@@ -2687,12 +2702,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>158</v>
+        <v>175</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>133</v>
@@ -2709,13 +2724,16 @@
       <c r="L74" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M74" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>141</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>158</v>
+        <v>175</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>135</v>
@@ -2732,16 +2750,19 @@
       <c r="L75" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M75" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>136</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>134</v>
@@ -2756,15 +2777,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>147</v>
+        <v>178</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>134</v>
@@ -2779,15 +2800,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>138</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>134</v>
@@ -2802,15 +2823,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>139</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>146</v>
+        <v>179</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>134</v>
@@ -2825,15 +2846,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>134</v>
@@ -2850,13 +2871,13 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B81" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F81" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="L81" s="1">
         <v>0</v>
@@ -2864,16 +2885,16 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B82" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F82" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F82" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="G82" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L82" s="1">
         <v>0</v>
@@ -2881,16 +2902,16 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B83" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F83" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F83" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="G83" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="L83" s="1">
         <v>0</v>
@@ -2898,16 +2919,16 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B84" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F84" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="L84" s="1">
         <v>0</v>
@@ -2915,16 +2936,16 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L85" s="1">
         <v>0</v>
@@ -2932,16 +2953,16 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B86" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F86" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F86" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="G86" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H86" s="1">
         <v>1</v>
@@ -2955,33 +2976,33 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L87" s="1">
         <v>106601</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B88" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F88" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="H88" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
update case about Work_Center3 with plant_owner=3
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-connector-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-backup\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65101437-4C43-4555-B68F-D0C06B4B09D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7112C22E-7340-43A5-9BF0-FC9D313082F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="181">
   <si>
     <t>name</t>
   </si>
@@ -575,11 +575,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>plant_owner=3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>do not support ruleKey value</t>
+    <t>plant_owner='3'</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -940,9 +936,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L75" sqref="L75"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M90" sqref="M90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2869,7 +2865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>159</v>
       </c>
@@ -2883,7 +2879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>160</v>
       </c>
@@ -2900,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>161</v>
       </c>
@@ -2917,7 +2913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>162</v>
       </c>
@@ -2934,7 +2930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>163</v>
       </c>
@@ -2951,7 +2947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>166</v>
       </c>
@@ -2974,7 +2970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>169</v>
       </c>
@@ -2988,13 +2984,10 @@
         <v>158</v>
       </c>
       <c r="L87" s="1">
-        <v>106601</v>
-      </c>
-      <c r="M87" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>170</v>
       </c>

</xml_diff>

<commit_message>
update_time of snc-test of clickhouse was string type update to use
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-connector-test-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4461EB01-4EA6-40EF-82EC-D1305C1ADE59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B464172-06C8-49C5-9C1E-F99BBDD2470E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="171">
   <si>
     <t>name</t>
   </si>
@@ -435,15 +435,6 @@
     <t>snc-connector-test-clickhouse-time-1</t>
   </si>
   <si>
-    <t>snc-connector-test-clickhouse-time-2</t>
-  </si>
-  <si>
-    <t>snc-connector-test-clickhouse-time-3</t>
-  </si>
-  <si>
-    <t>snc-connector-test-clickhouse-time-4</t>
-  </si>
-  <si>
     <t>snc-connector-test-clickhouse-int-1</t>
   </si>
   <si>
@@ -523,24 +514,12 @@
   </si>
   <si>
     <t>snc-connector-differentTablesInTwoDb-8</t>
-  </si>
-  <si>
-    <t>update_time&lt;'2021-09-06 13:33:58'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>update_time&lt;'2021-09-06T13:34:18'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>This entity 12321 is not found in domain [complexjson].</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>update_time&lt;'2021-06-03 04:50:19'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>plant_owner='3'</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -565,11 +544,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>update_time&lt;'2022-04-23T04:50:19'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SINAMICS_300_Log</t>
+    <t>update_time&lt;'1656038990'</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -928,11 +903,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
-  <dimension ref="A1:M87"/>
+  <dimension ref="A1:M84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A76" sqref="A76:XFD76"/>
+      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1080,7 +1055,7 @@
         <v>108002</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2077,7 +2052,7 @@
         <v>107</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>83</v>
@@ -2100,7 +2075,7 @@
         <v>108</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>85</v>
@@ -2123,7 +2098,7 @@
         <v>109</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>86</v>
@@ -2146,7 +2121,7 @@
         <v>110</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>88</v>
@@ -2169,7 +2144,7 @@
         <v>111</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>90</v>
@@ -2192,7 +2167,7 @@
         <v>112</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>92</v>
@@ -2215,7 +2190,7 @@
         <v>113</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>94</v>
@@ -2238,7 +2213,7 @@
         <v>114</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>96</v>
@@ -2261,7 +2236,7 @@
         <v>115</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>98</v>
@@ -2284,7 +2259,7 @@
         <v>116</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>100</v>
@@ -2307,7 +2282,7 @@
         <v>117</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>101</v>
@@ -2330,10 +2305,10 @@
         <v>118</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>25</v>
@@ -2350,13 +2325,13 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>25</v>
@@ -2373,10 +2348,10 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>102</v>
@@ -2399,7 +2374,7 @@
         <v>119</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>103</v>
@@ -2422,7 +2397,7 @@
         <v>120</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>104</v>
@@ -2445,10 +2420,10 @@
         <v>121</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>105</v>
@@ -2468,10 +2443,10 @@
         <v>122</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>105</v>
@@ -2491,10 +2466,10 @@
         <v>123</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>105</v>
@@ -2514,10 +2489,10 @@
         <v>124</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>105</v>
@@ -2537,10 +2512,10 @@
         <v>125</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>105</v>
@@ -2560,10 +2535,10 @@
         <v>126</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>105</v>
@@ -2583,7 +2558,7 @@
         <v>127</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>106</v>
@@ -2606,10 +2581,10 @@
         <v>128</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>87</v>
@@ -2629,10 +2604,10 @@
         <v>129</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>87</v>
@@ -2652,10 +2627,10 @@
         <v>130</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>87</v>
@@ -2675,10 +2650,10 @@
         <v>131</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>87</v>
@@ -2698,7 +2673,7 @@
         <v>132</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>133</v>
@@ -2718,13 +2693,13 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>134</v>
@@ -2744,10 +2719,10 @@
         <v>135</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>134</v>
@@ -2764,22 +2739,13 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H77" s="1">
-        <v>1</v>
-      </c>
-      <c r="I77" s="1">
-        <v>2</v>
+        <v>151</v>
       </c>
       <c r="L77" s="1">
         <v>0</v>
@@ -2787,22 +2753,16 @@
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="H78" s="1">
-        <v>1</v>
-      </c>
-      <c r="I78" s="1">
-        <v>2</v>
+        <v>151</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>157</v>
       </c>
       <c r="L78" s="1">
         <v>0</v>
@@ -2810,22 +2770,16 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H79" s="1">
-        <v>1</v>
-      </c>
-      <c r="I79" s="1">
-        <v>2</v>
+        <v>151</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="L79" s="1">
         <v>0</v>
@@ -2836,10 +2790,13 @@
         <v>155</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L80" s="1">
         <v>0</v>
@@ -2850,13 +2807,13 @@
         <v>156</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="L81" s="1">
         <v>0</v>
@@ -2864,16 +2821,22 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G82" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B82" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>163</v>
+      <c r="H82" s="1">
+        <v>1</v>
+      </c>
+      <c r="I82" s="1">
+        <v>2</v>
       </c>
       <c r="L82" s="1">
         <v>0</v>
@@ -2881,16 +2844,16 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L83" s="1">
         <v>0</v>
@@ -2898,78 +2861,21 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E84" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H84" s="1">
         <v>1</v>
       </c>
-      <c r="F84" s="1" t="s">
-        <v>154</v>
+      <c r="I84" s="1">
+        <v>2</v>
       </c>
       <c r="L84" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="H85" s="1">
-        <v>1</v>
-      </c>
-      <c r="I85" s="1">
-        <v>2</v>
-      </c>
-      <c r="L85" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="L86" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="H87" s="1">
-        <v>1</v>
-      </c>
-      <c r="I87" s="1">
-        <v>2</v>
-      </c>
-      <c r="L87" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>